<commit_message>
finish some little problem。perfect NO2
</commit_message>
<xml_diff>
--- a/3008播放器.xlsx
+++ b/3008播放器.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
   <si>
     <t>进度条不走动</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -298,6 +298,50 @@
   </si>
   <si>
     <t>2016.5.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优化一下代码，比如增加注释，对调试信息的管控、改善列表页面判断的顺序，对常量进行全局的管理，去掉一些没有用的代码等等。查找一下隐藏的bug。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一次进入无法全屏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.5.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>退出时，保存顶部和进度条隐藏的状态值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片界面一直处于加载界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>判断条件出错，一直无法进入刷新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成了调试信息的管控、全局变量进行了管理。其他未完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在播放视频的时候去看缩略图片，刷新显示的慢，在音乐界面就很快</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>估计是内存的占用问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>。。。。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -657,7 +701,8 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1109,39 +1154,77 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+    <row r="24" spans="1:9" ht="99" customHeight="1">
+      <c r="A24" s="1">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="1">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="A27" s="1">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>

</xml_diff>

<commit_message>
finish the zoom not smooth problem and load slow problem.
</commit_message>
<xml_diff>
--- a/3008播放器.xlsx
+++ b/3008播放器.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="96">
   <si>
     <t>进度条不走动</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -337,11 +337,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>估计是内存的占用问题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>。。。。</t>
+    <t>估计是内存的占用问题，图片加载效率还是太低了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不需要这个图片，要进行实时显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加载指定文件夹的图片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对查询出出来的图片进行判断</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gridview的setselection无效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大图的缩放问题，图片显示的不正常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>matrix图形变换，实现图片的缩放，效果比较好了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.5.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.5.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在每次点击item的时候，一直进行notifyDataSetChanged，这个严重影响了刷新的速度。去掉之后，在图片界面显示就比较快了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>莫名其妙就好了，也许真不应该加上notifyDataSetChanged。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>音乐暂停状态下，按下返回键，播放按钮上的暂停图片变成了播放图片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onbackpress函数中修改</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -388,12 +444,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -698,11 +757,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -710,6 +769,7 @@
     <col min="2" max="2" width="59.25" customWidth="1"/>
     <col min="3" max="3" width="55.875" customWidth="1"/>
     <col min="4" max="4" width="54.75" customWidth="1"/>
+    <col min="6" max="6" width="13.125" customWidth="1"/>
     <col min="7" max="7" width="26.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -741,11 +801,11 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -760,9 +820,9 @@
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="1" t="s">
         <v>41</v>
       </c>
@@ -775,9 +835,9 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
@@ -847,13 +907,13 @@
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -868,9 +928,9 @@
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="1" t="s">
         <v>22</v>
       </c>
@@ -942,10 +1002,12 @@
       <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="3" t="s">
-        <v>54</v>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>33</v>
@@ -1211,7 +1273,7 @@
       </c>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" ht="45" customHeight="1">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -1221,12 +1283,84 @@
       <c r="C27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="E27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="1">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
finish the problem when in shunxu playmode,and play finish the last item
</commit_message>
<xml_diff>
--- a/3008播放器.xlsx
+++ b/3008播放器.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="122">
   <si>
     <t>问题</t>
   </si>
@@ -132,246 +132,288 @@
     <t>清除flag，强制系统UI全屏</t>
   </si>
   <si>
+    <t>ANR</t>
+  </si>
+  <si>
+    <t>程序加载工程中出现出现白屏现象</t>
+  </si>
+  <si>
+    <t>白屏现象，主要是由于加载的时间过长，出现了短暂的白屏现象。</t>
+  </si>
+  <si>
+    <t>给出了加载界面，那么就考虑把所有的加载工作放在列表界面进行。在程序进入的时候，开启子线程进行数据加载。当用户点击列表的时候，看加载状态来判定界面。白屏是数据的程序的一些初始化数据的加载，可以通过修改theme，来改变这个背景，但是这个过程暂时没办法消除，后期可以继续优化。</t>
+  </si>
+  <si>
+    <t>2016.5.6</t>
+  </si>
+  <si>
+    <t>体验问题、效率问题</t>
+  </si>
+  <si>
+    <t>后期继续优化</t>
+  </si>
+  <si>
+    <t>程序退出之后的记忆功能没有</t>
+  </si>
+  <si>
+    <t>考虑好需要记录哪些东西</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1、退出程序时候的最后一个音乐程序信息（sharepreference）。2、及记录所有视频的已经播放的时间(所有信息的记录之后，再次进入需要判定所有资源是否还存在。)                                                     </t>
+  </si>
+  <si>
+    <t>体验问题</t>
+  </si>
+  <si>
+    <t>程序按下返回键之后，再回来屏幕是黑色的。</t>
+  </si>
+  <si>
+    <t>需要将屏幕暂停到之前的播放进度上去，界面显示到相应的图片暂停</t>
+  </si>
+  <si>
+    <t>2016.5.7</t>
+  </si>
+  <si>
+    <t>音频焦点</t>
+  </si>
+  <si>
+    <t>在每次进行播放的时候才请求获取音频焦点</t>
+  </si>
+  <si>
+    <t>视频焦点</t>
+  </si>
+  <si>
+    <t>每次mainacitvity resume的时候，都进行焦点获取</t>
+  </si>
+  <si>
+    <t>播放视频的时候去加载图片，很慢</t>
+  </si>
+  <si>
+    <t>主要是内存问题。</t>
+  </si>
+  <si>
+    <t>优化一下代码，比如增加注释，对调试信息的管控、改善列表页面判断的顺序，对常量进行全局的管理，去掉一些没有用的代码等等。查找一下隐藏的bug。</t>
+  </si>
+  <si>
+    <t>完成了调试信息的管控、全局变量进行了管理。其他未完成</t>
+  </si>
+  <si>
+    <t>第一次进入无法全屏</t>
+  </si>
+  <si>
+    <t>退出时，保存顶部和进度条隐藏的状态值</t>
+  </si>
+  <si>
+    <t>图片界面一直处于加载界面</t>
+  </si>
+  <si>
+    <t>判断条件出错，一直无法进入刷新</t>
+  </si>
+  <si>
+    <t>在播放视频的时候去看缩略图片，刷新显示的慢，在音乐界面就很快</t>
+  </si>
+  <si>
+    <t>在每次点击item的时候，一直进行notifyDataSetChanged，这个严重影响了刷新的速度。去掉之后，在图片界面显示就比较快了。</t>
+  </si>
+  <si>
+    <t>2016.5.10</t>
+  </si>
+  <si>
+    <t>加载指定文件夹的图片</t>
+  </si>
+  <si>
+    <t>对查询出出来的图片进行判断</t>
+  </si>
+  <si>
+    <t>gridview的setselection无效</t>
+  </si>
+  <si>
+    <t>莫名其妙就好了，也许真不应该加上notifyDataSetChanged。</t>
+  </si>
+  <si>
+    <t>大图的缩放问题，图片显示的不正常</t>
+  </si>
+  <si>
+    <t>matrix图形变换，实现图片的缩放，效果比较好了</t>
+  </si>
+  <si>
+    <t>音乐暂停状态下，按下返回键，播放按钮上的暂停图片变成了播放图片</t>
+  </si>
+  <si>
+    <t>onbackpress函数中修改</t>
+  </si>
+  <si>
+    <t>超过一个小时以上的时间显示问题</t>
+  </si>
+  <si>
+    <t>时间计算出错了，修正就可以了</t>
+  </si>
+  <si>
+    <t>2016.5.11</t>
+  </si>
+  <si>
+    <t>usb检测带来的问题</t>
+  </si>
+  <si>
+    <t>压力测试</t>
+  </si>
+  <si>
+    <t>还有压力测试，U盘异常退出该怎么处理</t>
+  </si>
+  <si>
+    <t>mp3infos在activity和服务中不是同一个，且赋值出错</t>
+  </si>
+  <si>
+    <t>一边扫描，一边播放音乐</t>
+  </si>
+  <si>
+    <t>在没有unmount状态下，为什么列表会出现扫描的状态</t>
+  </si>
+  <si>
+    <t>一边扫描，一边播放的时候，音乐界面如何刷新</t>
+  </si>
+  <si>
+    <t>数据刷新的地方？</t>
+  </si>
+  <si>
+    <t>message、点击列表按钮、点击音频、视频、图片按钮</t>
+  </si>
+  <si>
+    <t>数据刷新的时间？</t>
+  </si>
+  <si>
+    <t>不应该以ifmusicloaded的状态来改变图片背景，应该以u盘的状态和是否扫描出来了数据为判断依据。</t>
+  </si>
+  <si>
+    <t>上一次数据的加载</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>usb检测问题，通过广播，只能获取到是否有u盘存在，无法知道mediastore是否全部写入完毕，通过video项目中的一个服务，可以获取状态值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当播放状态关机，重启后，马上去启动程序，这个时候，依然是scan状态，但是收不到scan的广播，所以我就没有去判断是否和以前一样了(和以前一样，加载上次数据的前提是，进入就是finish状态)。并且由于收不到scan，只能等待finish的时候去加载数据，这期间等待的时间也是比较长的。考虑状态值是否要多一个scan的状态值判断？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.5.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自己的判断条件出错</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>思路参考</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲突原因是，在加载过程中，我肯定是要在ui界面上显示数据的，开始可能加载的不是上次记录的数据，所以要用加载的第一个数据来替代，但是有一个问题，后面上次记录的数据出来了，该怎么处理？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开机可能scan状态下，就启动程序了，关于上次记录数据，与本次加载数据的过程中的数据冲突？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>估计是内存的占用问题，图片加载效率还是太低了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进行播放，忘记修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>改善思路：扫描的过程中，让current_music_num一直为-1，并且点击播放、上下曲目，不能播放。除非用户在扫描过程中点击了播放列表的item。且不进行ui界面的刷新，如果扫描完了current_music_num还是等于-1，这个时候判断是否有和之前记录的current_musci_num相等的，若是，赋值。否则让current_music_num为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U盘异常退出，程序应该获取一个unmounted，得到消息后，提示用户程序退出。3s后自动退出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>共同维护baseapp中的mp3infos，删除了mainacitivity的mp3infos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看usb逻辑文档，在scanstart时，就扫描，然后进行定时器扫描</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>usb检测</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getstate只能获取scan start和scan finish的两种状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过加入路径的判断，判断四种u盘状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.5.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>把第一首歌刷新出来，然后就是曲目要变化，还是等全部刷新完毕后，把前一次记录的音乐刷新出来？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参看42点的更新思路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>视频模块，顺序播放到最后一个曲目了之后，暂停按钮没有改变过来</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当列表open的时候，曲目变成了下一曲的时候，列表没有刷新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机播放似乎没有器作用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>顺序播放，到最后一首歌的时候，停了下来，手动滑动滑动条，按钮变化了，但是没有播放歌曲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>视频模块，到最后一视频的时候，停了下来，手动滑动滑动条，按钮无变化了，也没有进行播放</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>改变服务中的停止，为暂停</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口回调，刷新list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口回调，修改播放按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.5.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>全屏后，按返回键，出现anr</t>
-  </si>
-  <si>
-    <t>ANR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>重新创建的时候，自己设置成了FLAG_NOT_FOCUS.更改即可</t>
-  </si>
-  <si>
-    <t>程序加载工程中出现出现白屏现象</t>
-  </si>
-  <si>
-    <t>白屏现象，主要是由于加载的时间过长，出现了短暂的白屏现象。</t>
-  </si>
-  <si>
-    <t>给出了加载界面，那么就考虑把所有的加载工作放在列表界面进行。在程序进入的时候，开启子线程进行数据加载。当用户点击列表的时候，看加载状态来判定界面。白屏是数据的程序的一些初始化数据的加载，可以通过修改theme，来改变这个背景，但是这个过程暂时没办法消除，后期可以继续优化。</t>
-  </si>
-  <si>
-    <t>2016.5.6</t>
-  </si>
-  <si>
-    <t>体验问题、效率问题</t>
-  </si>
-  <si>
-    <t>后期继续优化</t>
-  </si>
-  <si>
-    <t>程序退出之后的记忆功能没有</t>
-  </si>
-  <si>
-    <t>考虑好需要记录哪些东西</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1、退出程序时候的最后一个音乐程序信息（sharepreference）。2、及记录所有视频的已经播放的时间(所有信息的记录之后，再次进入需要判定所有资源是否还存在。)                                                     </t>
-  </si>
-  <si>
-    <t>体验问题</t>
-  </si>
-  <si>
-    <t>程序按下返回键之后，再回来屏幕是黑色的。</t>
-  </si>
-  <si>
-    <t>需要将屏幕暂停到之前的播放进度上去，界面显示到相应的图片暂停</t>
-  </si>
-  <si>
-    <t>2016.5.7</t>
-  </si>
-  <si>
-    <t>音频焦点</t>
-  </si>
-  <si>
-    <t>在每次进行播放的时候才请求获取音频焦点</t>
-  </si>
-  <si>
-    <t>视频焦点</t>
-  </si>
-  <si>
-    <t>每次mainacitvity resume的时候，都进行焦点获取</t>
-  </si>
-  <si>
-    <t>播放视频的时候去加载图片，很慢</t>
-  </si>
-  <si>
-    <t>主要是内存问题。</t>
-  </si>
-  <si>
-    <t>优化一下代码，比如增加注释，对调试信息的管控、改善列表页面判断的顺序，对常量进行全局的管理，去掉一些没有用的代码等等。查找一下隐藏的bug。</t>
-  </si>
-  <si>
-    <t>完成了调试信息的管控、全局变量进行了管理。其他未完成</t>
-  </si>
-  <si>
-    <t>第一次进入无法全屏</t>
-  </si>
-  <si>
-    <t>退出时，保存顶部和进度条隐藏的状态值</t>
-  </si>
-  <si>
-    <t>图片界面一直处于加载界面</t>
-  </si>
-  <si>
-    <t>判断条件出错，一直无法进入刷新</t>
-  </si>
-  <si>
-    <t>在播放视频的时候去看缩略图片，刷新显示的慢，在音乐界面就很快</t>
-  </si>
-  <si>
-    <t>在每次点击item的时候，一直进行notifyDataSetChanged，这个严重影响了刷新的速度。去掉之后，在图片界面显示就比较快了。</t>
-  </si>
-  <si>
-    <t>2016.5.10</t>
-  </si>
-  <si>
-    <t>加载指定文件夹的图片</t>
-  </si>
-  <si>
-    <t>对查询出出来的图片进行判断</t>
-  </si>
-  <si>
-    <t>gridview的setselection无效</t>
-  </si>
-  <si>
-    <t>莫名其妙就好了，也许真不应该加上notifyDataSetChanged。</t>
-  </si>
-  <si>
-    <t>大图的缩放问题，图片显示的不正常</t>
-  </si>
-  <si>
-    <t>matrix图形变换，实现图片的缩放，效果比较好了</t>
-  </si>
-  <si>
-    <t>音乐暂停状态下，按下返回键，播放按钮上的暂停图片变成了播放图片</t>
-  </si>
-  <si>
-    <t>onbackpress函数中修改</t>
-  </si>
-  <si>
-    <t>超过一个小时以上的时间显示问题</t>
-  </si>
-  <si>
-    <t>时间计算出错了，修正就可以了</t>
-  </si>
-  <si>
-    <t>2016.5.11</t>
-  </si>
-  <si>
-    <t>usb检测带来的问题</t>
-  </si>
-  <si>
-    <t>压力测试</t>
-  </si>
-  <si>
-    <t>还有压力测试，U盘异常退出该怎么处理</t>
-  </si>
-  <si>
-    <t>mp3infos在activity和服务中不是同一个，且赋值出错</t>
-  </si>
-  <si>
-    <t>一边扫描，一边播放音乐</t>
-  </si>
-  <si>
-    <t>在没有unmount状态下，为什么列表会出现扫描的状态</t>
-  </si>
-  <si>
-    <t>一边扫描，一边播放的时候，音乐界面如何刷新</t>
-  </si>
-  <si>
-    <t>数据刷新的地方？</t>
-  </si>
-  <si>
-    <t>message、点击列表按钮、点击音频、视频、图片按钮</t>
-  </si>
-  <si>
-    <t>数据刷新的时间？</t>
-  </si>
-  <si>
-    <t>不应该以ifmusicloaded的状态来改变图片背景，应该以u盘的状态和是否扫描出来了数据为判断依据。</t>
-  </si>
-  <si>
-    <t>上一次数据的加载</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>usb检测问题，通过广播，只能获取到是否有u盘存在，无法知道mediastore是否全部写入完毕，通过video项目中的一个服务，可以获取状态值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>当播放状态关机，重启后，马上去启动程序，这个时候，依然是scan状态，但是收不到scan的广播，所以我就没有去判断是否和以前一样了(和以前一样，加载上次数据的前提是，进入就是finish状态)。并且由于收不到scan，只能等待finish的时候去加载数据，这期间等待的时间也是比较长的。考虑状态值是否要多一个scan的状态值判断？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ok</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2015.5.12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自己的判断条件出错</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>思路参考</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>冲突原因是，在加载过程中，我肯定是要在ui界面上显示数据的，开始可能加载的不是上次记录的数据，所以要用加载的第一个数据来替代，但是有一个问题，后面上次记录的数据出来了，该怎么处理？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>开机可能scan状态下，就启动程序了，关于上次记录数据，与本次加载数据的过程中的数据冲突？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>估计是内存的占用问题，图片加载效率还是太低了。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>进行播放，忘记修改</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>改善思路：扫描的过程中，让current_music_num一直为-1，并且点击播放、上下曲目，不能播放。除非用户在扫描过程中点击了播放列表的item。且不进行ui界面的刷新，如果扫描完了current_music_num还是等于-1，这个时候判断是否有和之前记录的current_musci_num相等的，若是，赋值。否则让current_music_num为0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>U盘异常退出，程序应该获取一个unmounted，得到消息后，提示用户程序退出。3s后自动退出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>共同维护baseapp中的mp3infos，删除了mainacitivity的mp3infos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>看usb逻辑文档，在scanstart时，就扫描，然后进行定时器扫描</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>usb检测</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>getstate只能获取scan start和scan finish的两种状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过加入路径的判断，判断四种u盘状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2015.5.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>把第一首歌刷新出来，然后就是曲目要变化，还是等全部刷新完毕后，把前一次记录的音乐刷新出来？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>参看42点的更新思路</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -416,7 +458,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -440,6 +482,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,11 +780,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C33:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -779,11 +824,11 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -798,9 +843,9 @@
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
@@ -813,9 +858,9 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
@@ -847,7 +892,7 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>8</v>
@@ -885,13 +930,13 @@
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -906,9 +951,9 @@
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1036,14 +1081,14 @@
       <c r="A16" s="1">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>40</v>
+      <c r="D16" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>34</v>
@@ -1058,25 +1103,25 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -1085,43 +1130,43 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="27">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1129,17 +1174,17 @@
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1148,17 +1193,17 @@
         <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1167,10 +1212,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
@@ -1182,17 +1227,17 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1201,17 +1246,17 @@
         <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -1220,17 +1265,17 @@
         <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -1239,19 +1284,19 @@
         <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -1260,16 +1305,16 @@
         <v>28</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1277,16 +1322,16 @@
         <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1294,16 +1339,16 @@
         <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1311,16 +1356,16 @@
         <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1328,43 +1373,43 @@
         <v>32</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A32" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="A32" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:7" ht="57.75" customHeight="1">
       <c r="A33" s="1">
         <v>33</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="F33" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="57.75" customHeight="1">
@@ -1372,19 +1417,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="69.75" customHeight="1">
@@ -1392,22 +1437,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="27">
@@ -1415,16 +1460,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1432,13 +1477,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="31.5" customHeight="1">
@@ -1446,16 +1491,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="27">
@@ -1463,19 +1508,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1483,13 +1528,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
@@ -1499,10 +1544,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
@@ -1513,10 +1558,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
@@ -1528,19 +1573,95 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="3">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="27">
+      <c r="A45" s="3">
+        <v>43</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="3">
+        <v>45</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="27">
+      <c r="A48" s="3">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" t="s">
+        <v>115</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>